<commit_message>
Scripts for wikipedia parsing
</commit_message>
<xml_diff>
--- a/Rulers/СССР.xlsx
+++ b/Rulers/СССР.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="207">
   <si>
     <t>person</t>
   </si>
@@ -184,36 +184,21 @@
     <t>Юрий Владимирович Андропов</t>
   </si>
   <si>
-    <t>Q121998</t>
+    <t>Q1048744</t>
+  </si>
+  <si>
+    <t>Q1959942</t>
+  </si>
+  <si>
+    <t>Q462189</t>
   </si>
   <si>
     <t>Q15628644</t>
   </si>
   <si>
-    <t>Q1048744</t>
-  </si>
-  <si>
-    <t>Q1959942</t>
-  </si>
-  <si>
-    <t>Q5452917</t>
-  </si>
-  <si>
-    <t>Q462189</t>
-  </si>
-  <si>
     <t>Q4376674</t>
   </si>
   <si>
-    <t>Q27491113</t>
-  </si>
-  <si>
-    <t>Q17276321</t>
-  </si>
-  <si>
-    <t>Q19399742</t>
-  </si>
-  <si>
     <t>Q2367317</t>
   </si>
   <si>
@@ -226,21 +211,9 @@
     <t>Q61899333</t>
   </si>
   <si>
-    <t>Q56919889</t>
-  </si>
-  <si>
-    <t>Q12155588</t>
-  </si>
-  <si>
     <t>Q2355240</t>
   </si>
   <si>
-    <t>Q40032487</t>
-  </si>
-  <si>
-    <t>Q4374313</t>
-  </si>
-  <si>
     <t>Q61870366</t>
   </si>
   <si>
@@ -259,42 +232,24 @@
     <t>Q4376657</t>
   </si>
   <si>
-    <t>Q75610609</t>
-  </si>
-  <si>
     <t>Q4376665</t>
   </si>
   <si>
-    <t>посол</t>
+    <t>генеральный секретарь ЦК КПСС</t>
+  </si>
+  <si>
+    <t>Министерство иностранных дел СССР</t>
+  </si>
+  <si>
+    <t>Главы правительства СССР</t>
   </si>
   <si>
     <t>депутат Верховного Совета СССР</t>
   </si>
   <si>
-    <t>генеральный секретарь ЦК КПСС</t>
-  </si>
-  <si>
-    <t>Министерство иностранных дел СССР</t>
-  </si>
-  <si>
-    <t>первый заместитель председателя Совета Министров СССР</t>
-  </si>
-  <si>
-    <t>Главы правительства СССР</t>
-  </si>
-  <si>
     <t>председатель Совета министров СССР</t>
   </si>
   <si>
-    <t>член Всероссийского Учредительного собрания</t>
-  </si>
-  <si>
-    <t>депутат Государственной думы РФ</t>
-  </si>
-  <si>
-    <t>член Совета Федерации</t>
-  </si>
-  <si>
     <t>Главы военного ведомства СССР</t>
   </si>
   <si>
@@ -307,21 +262,9 @@
     <t>председатель Совета Труда и Обороны СССР</t>
   </si>
   <si>
-    <t>председатель Совета народных комиссаров РСФСР</t>
-  </si>
-  <si>
-    <t>список первых секретарей ЦК Коммунистической партии Украины</t>
-  </si>
-  <si>
     <t>председатель Президиума Верховного Совета СССР</t>
   </si>
   <si>
-    <t>посол СССР в США</t>
-  </si>
-  <si>
-    <t>постоянный представитель Российской Федерации при Организации Объединённых Наций</t>
-  </si>
-  <si>
     <t>председатель Центрального исполнительного комитета СССР</t>
   </si>
   <si>
@@ -340,48 +283,33 @@
     <t>председатель Верховного Совета СССР</t>
   </si>
   <si>
-    <t>ambassador of the Soviet Union to Hungary</t>
-  </si>
-  <si>
     <t>председатель Комитета государственной безопасности СССР</t>
   </si>
   <si>
+    <t>1921-03-16T00:00:00Z</t>
+  </si>
+  <si>
+    <t>1953-03-05T00:00:00Z</t>
+  </si>
+  <si>
+    <t>1930-12-19T00:00:00Z</t>
+  </si>
+  <si>
     <t>не указано</t>
   </si>
   <si>
-    <t>1921-03-16T00:00:00Z</t>
-  </si>
-  <si>
-    <t>1953-03-05T00:00:00Z</t>
-  </si>
-  <si>
-    <t>1942-08-16T00:00:00Z</t>
-  </si>
-  <si>
-    <t>1930-12-19T00:00:00Z</t>
-  </si>
-  <si>
     <t>1953-03-06T00:00:00Z</t>
   </si>
   <si>
     <t>1964-10-15T00:00:00Z</t>
   </si>
   <si>
-    <t>1960-05-04T00:00:00Z</t>
-  </si>
-  <si>
     <t>1924-01-21T00:00:00Z</t>
   </si>
   <si>
     <t>1980-10-23T00:00:00Z</t>
   </si>
   <si>
-    <t>1976-09-02T00:00:00Z</t>
-  </si>
-  <si>
-    <t>2003-09-17T00:00:00Z</t>
-  </si>
-  <si>
     <t>1985-09-27T00:00:00Z</t>
   </si>
   <si>
@@ -406,15 +334,9 @@
     <t>1923-07-17T00:00:00Z</t>
   </si>
   <si>
-    <t>1917-11-09T00:00:00Z</t>
-  </si>
-  <si>
     <t>1953-09-14T00:00:00Z</t>
   </si>
   <si>
-    <t>1947-12-26T00:00:00Z</t>
-  </si>
-  <si>
     <t>1958-03-27T00:00:00Z</t>
   </si>
   <si>
@@ -424,21 +346,12 @@
     <t>1984-02-13T00:00:00Z</t>
   </si>
   <si>
-    <t>1955-02-28T00:00:00Z</t>
-  </si>
-  <si>
     <t>1964-07-15T00:00:00Z</t>
   </si>
   <si>
     <t>1985-07-02T00:00:00Z</t>
   </si>
   <si>
-    <t>1983-03-24T00:00:00Z</t>
-  </si>
-  <si>
-    <t>1946-04-01T00:00:00Z</t>
-  </si>
-  <si>
     <t>1925-11-06T00:00:00Z</t>
   </si>
   <si>
@@ -463,9 +376,6 @@
     <t>1954-01-01T00:00:00Z</t>
   </si>
   <si>
-    <t>1957-12-26T00:00:00Z</t>
-  </si>
-  <si>
     <t>1984-02-09T00:00:00Z</t>
   </si>
   <si>
@@ -514,9 +424,6 @@
     <t>http://www.wikidata.org/value/c121c28eba5b707f1f0425cdb5c84b75</t>
   </si>
   <si>
-    <t>http://www.wikidata.org/value/0fce3c0ccf7a2d29b4b8376540840ba4</t>
-  </si>
-  <si>
     <t>http://www.wikidata.org/value/679bcb6e943ee11bfc1b66e07129a519</t>
   </si>
   <si>
@@ -526,21 +433,12 @@
     <t>http://www.wikidata.org/value/d13532fdd7f8e90a0ffa82ebb43afd62</t>
   </si>
   <si>
-    <t>http://www.wikidata.org/value/78a52948cdb3ad8201690a99cad7e991</t>
-  </si>
-  <si>
     <t>http://www.wikidata.org/value/20359880cd0860bbe92bd364faa31f67</t>
   </si>
   <si>
     <t>http://www.wikidata.org/value/c4dc1083ef50545048818a59cfa06699</t>
   </si>
   <si>
-    <t>http://www.wikidata.org/value/6f941c42c1e8e9b14465a2f830be1ae2</t>
-  </si>
-  <si>
-    <t>http://www.wikidata.org/value/b9e85b2f8be9d7073fd34a934d268dff</t>
-  </si>
-  <si>
     <t>http://www.wikidata.org/value/229b6150c91d972579adb71fb1254718</t>
   </si>
   <si>
@@ -565,15 +463,9 @@
     <t>http://www.wikidata.org/value/78b18c6c8859bd48822841287c4efaf5</t>
   </si>
   <si>
-    <t>http://www.wikidata.org/value/4e0ff8562ddb9f0e0126f1795ba1a0dd</t>
-  </si>
-  <si>
     <t>http://www.wikidata.org/value/827d08d48bc2dd14e072013ed3771e3f</t>
   </si>
   <si>
-    <t>http://www.wikidata.org/value/d6a8232cc77d73d2b8649b3a7ffdc097</t>
-  </si>
-  <si>
     <t>http://www.wikidata.org/value/8b32492b0e8af7e23cc44f66b083812d</t>
   </si>
   <si>
@@ -583,21 +475,12 @@
     <t>http://www.wikidata.org/value/134dfc295889f0b8b14579e2e0bbe63b</t>
   </si>
   <si>
-    <t>http://www.wikidata.org/value/e1e1c7a7e3488b6eacef8dd810847be0</t>
-  </si>
-  <si>
     <t>http://www.wikidata.org/value/054aa9dcbcd78609457242154da7269c</t>
   </si>
   <si>
     <t>http://www.wikidata.org/value/0ab05ed2dfd8687d7947f5465a4ad1d5</t>
   </si>
   <si>
-    <t>http://www.wikidata.org/value/10afbfdbd9b3b5f51fa95ce4adffe09e</t>
-  </si>
-  <si>
-    <t>http://www.wikidata.org/value/191bc6c909a1a63e4ba839bbd01c79e5</t>
-  </si>
-  <si>
     <t>http://www.wikidata.org/value/4b8b9ffc9992cb9468b6994af7806542</t>
   </si>
   <si>
@@ -622,9 +505,6 @@
     <t>http://www.wikidata.org/value/9adc78d0b1f8e9bff61cdffaddf4e606</t>
   </si>
   <si>
-    <t>http://www.wikidata.org/value/833af58451041c1d7f3a48cd05c69b52</t>
-  </si>
-  <si>
     <t>http://www.wikidata.org/value/9d5f2faeb08c274f5cbe3ce25fe321a8</t>
   </si>
   <si>
@@ -670,9 +550,6 @@
     <t>1956-06-01T00:00:00Z</t>
   </si>
   <si>
-    <t>1957-06-29T00:00:00Z</t>
-  </si>
-  <si>
     <t>1955-02-08T00:00:00Z</t>
   </si>
   <si>
@@ -691,12 +568,6 @@
     <t>1952-10-16T00:00:00Z</t>
   </si>
   <si>
-    <t>1949-12-19T00:00:00Z</t>
-  </si>
-  <si>
-    <t>1948-01-01T00:00:00Z</t>
-  </si>
-  <si>
     <t>1940-05-07T00:00:00Z</t>
   </si>
   <si>
@@ -709,9 +580,6 @@
     <t>1977-01-01T00:00:00Z</t>
   </si>
   <si>
-    <t>1963-07-02T00:00:00Z</t>
-  </si>
-  <si>
     <t>1946-02-10T00:00:00Z</t>
   </si>
   <si>
@@ -721,15 +589,9 @@
     <t>1991-08-24T00:00:00Z</t>
   </si>
   <si>
-    <t>1957-01-01T00:00:00Z</t>
-  </si>
-  <si>
     <t>http://www.wikidata.org/value/10b62e196e0f6f7ed4883db2a8247a36</t>
   </si>
   <si>
-    <t>http://www.wikidata.org/value/9218f6becc94c61b8b030be6fa2b0686</t>
-  </si>
-  <si>
     <t>http://www.wikidata.org/value/5ea39264ab9722290f81d25daad9e295</t>
   </si>
   <si>
@@ -748,12 +610,6 @@
     <t>http://www.wikidata.org/value/2824431a13657ecf44ac5656ed7432b0</t>
   </si>
   <si>
-    <t>http://www.wikidata.org/value/0f816c80d6c31bdeb315f2493930c82b</t>
-  </si>
-  <si>
-    <t>http://www.wikidata.org/value/ec8eae08c5ae82941e89496436677d0e</t>
-  </si>
-  <si>
     <t>http://www.wikidata.org/value/a9eb2350df7826185b6b1e5005f247c8</t>
   </si>
   <si>
@@ -766,9 +622,6 @@
     <t>http://www.wikidata.org/value/749910ebd6c8faae3d32b17def13c5bd</t>
   </si>
   <si>
-    <t>http://www.wikidata.org/value/339df9e86ac9ce417ebd651944b5f6c6</t>
-  </si>
-  <si>
     <t>http://www.wikidata.org/value/cfdcec77a4ac11d1773a41c54ee1fba4</t>
   </si>
   <si>
@@ -778,7 +631,7 @@
     <t>http://www.wikidata.org/value/ea3a4611e96955d10a2f7bef2726cc70</t>
   </si>
   <si>
-    <t>http://www.wikidata.org/value/3ce9f606decac48214dd1c61f4d5e37d</t>
+    <t>T</t>
   </si>
   <si>
     <t>F</t>
@@ -1152,7 +1005,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J79"/>
+  <dimension ref="A1:J61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1201,25 +1054,25 @@
         <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="E2" t="s">
-        <v>110</v>
-      </c>
-      <c r="F2" t="s">
-        <v>110</v>
+        <v>90</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>134</v>
       </c>
       <c r="G2" t="s">
-        <v>110</v>
-      </c>
-      <c r="H2" t="s">
-        <v>110</v>
+        <v>103</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>146</v>
       </c>
       <c r="I2" t="s">
-        <v>255</v>
+        <v>205</v>
       </c>
       <c r="J2" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1233,25 +1086,25 @@
         <v>57</v>
       </c>
       <c r="D3" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="E3" t="s">
-        <v>110</v>
-      </c>
-      <c r="F3" t="s">
-        <v>110</v>
+        <v>91</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="G3" t="s">
-        <v>110</v>
-      </c>
-      <c r="H3" t="s">
-        <v>110</v>
+        <v>177</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>191</v>
       </c>
       <c r="I3" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J3" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -1265,25 +1118,25 @@
         <v>58</v>
       </c>
       <c r="D4" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="E4" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>164</v>
+        <v>136</v>
       </c>
       <c r="G4" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>180</v>
+        <v>144</v>
       </c>
       <c r="I4" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J4" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -1297,89 +1150,89 @@
         <v>59</v>
       </c>
       <c r="D5" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="E5" t="s">
-        <v>112</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>165</v>
+        <v>93</v>
+      </c>
+      <c r="F5" t="s">
+        <v>93</v>
       </c>
       <c r="G5" t="s">
-        <v>217</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>236</v>
+        <v>93</v>
+      </c>
+      <c r="H5" t="s">
+        <v>93</v>
       </c>
       <c r="I5" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J5" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D6" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="E6" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>166</v>
+        <v>137</v>
       </c>
       <c r="G6" t="s">
-        <v>218</v>
+        <v>178</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>237</v>
+        <v>192</v>
       </c>
       <c r="I6" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J6" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D7" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="E7" t="s">
-        <v>114</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>167</v>
+        <v>93</v>
+      </c>
+      <c r="F7" t="s">
+        <v>93</v>
       </c>
       <c r="G7" t="s">
-        <v>125</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>178</v>
+        <v>93</v>
+      </c>
+      <c r="H7" t="s">
+        <v>93</v>
       </c>
       <c r="I7" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J7" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -1390,92 +1243,92 @@
         <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D8" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="E8" t="s">
-        <v>115</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>168</v>
+        <v>93</v>
+      </c>
+      <c r="F8" t="s">
+        <v>93</v>
       </c>
       <c r="G8" t="s">
-        <v>219</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>238</v>
+        <v>93</v>
+      </c>
+      <c r="H8" t="s">
+        <v>93</v>
       </c>
       <c r="I8" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J8" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D9" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="E9" t="s">
-        <v>110</v>
-      </c>
-      <c r="F9" t="s">
-        <v>110</v>
+        <v>95</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="G9" t="s">
-        <v>110</v>
-      </c>
-      <c r="H9" t="s">
-        <v>110</v>
+        <v>97</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>140</v>
       </c>
       <c r="I9" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J9" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D10" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="E10" t="s">
-        <v>110</v>
-      </c>
-      <c r="F10" t="s">
-        <v>110</v>
+        <v>95</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="G10" t="s">
-        <v>110</v>
-      </c>
-      <c r="H10" t="s">
-        <v>110</v>
+        <v>97</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>140</v>
       </c>
       <c r="I10" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J10" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="11" spans="1:10">
@@ -1486,2224 +1339,1648 @@
         <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D11" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E11" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="F11" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="G11" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="H11" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="I11" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J11" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D12" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="E12" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>169</v>
+        <v>139</v>
       </c>
       <c r="G12" t="s">
-        <v>119</v>
+        <v>179</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>172</v>
+        <v>193</v>
       </c>
       <c r="I12" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J12" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
         <v>60</v>
       </c>
       <c r="D13" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="E13" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>170</v>
+        <v>140</v>
       </c>
       <c r="G13" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>169</v>
+        <v>141</v>
       </c>
       <c r="I13" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J13" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D14" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="E14" t="s">
-        <v>116</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>169</v>
+        <v>93</v>
+      </c>
+      <c r="F14" t="s">
+        <v>93</v>
       </c>
       <c r="G14" t="s">
-        <v>119</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>172</v>
+        <v>93</v>
+      </c>
+      <c r="H14" t="s">
+        <v>93</v>
       </c>
       <c r="I14" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J14" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D15" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="E15" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>171</v>
+        <v>141</v>
       </c>
       <c r="G15" t="s">
-        <v>220</v>
+        <v>99</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>239</v>
+        <v>142</v>
       </c>
       <c r="I15" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J15" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C16" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D16" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="E16" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="F16" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="G16" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="H16" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="I16" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J16" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D17" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="E17" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>172</v>
+        <v>142</v>
       </c>
       <c r="G17" t="s">
-        <v>122</v>
+        <v>180</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>175</v>
+        <v>194</v>
       </c>
       <c r="I17" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J17" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D18" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="E18" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>173</v>
+        <v>143</v>
       </c>
       <c r="G18" t="s">
-        <v>119</v>
+        <v>181</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>172</v>
+        <v>195</v>
       </c>
       <c r="I18" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J18" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D19" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E19" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="F19" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="G19" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="H19" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="I19" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J19" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C20" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D20" t="s">
+        <v>75</v>
+      </c>
+      <c r="E20" t="s">
+        <v>101</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G20" t="s">
         <v>91</v>
       </c>
-      <c r="E20" t="s">
-        <v>121</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="G20" t="s">
-        <v>121</v>
-      </c>
       <c r="H20" s="2" t="s">
-        <v>174</v>
+        <v>135</v>
       </c>
       <c r="I20" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J20" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D21" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="E21" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>175</v>
+        <v>145</v>
       </c>
       <c r="G21" t="s">
-        <v>123</v>
+        <v>182</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>176</v>
+        <v>196</v>
       </c>
       <c r="I21" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J21" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D22" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="E22" t="s">
-        <v>110</v>
-      </c>
-      <c r="F22" t="s">
-        <v>110</v>
+        <v>103</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>146</v>
       </c>
       <c r="G22" t="s">
-        <v>110</v>
-      </c>
-      <c r="H22" t="s">
-        <v>110</v>
+        <v>183</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>197</v>
       </c>
       <c r="I22" t="s">
-        <v>255</v>
+        <v>205</v>
       </c>
       <c r="J22" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C23" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D23" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="E23" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="F23" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="G23" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="H23" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="I23" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J23" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C24" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D24" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="E24" t="s">
-        <v>123</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>176</v>
+        <v>93</v>
+      </c>
+      <c r="F24" t="s">
+        <v>93</v>
       </c>
       <c r="G24" t="s">
-        <v>221</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>240</v>
+        <v>93</v>
+      </c>
+      <c r="H24" t="s">
+        <v>93</v>
       </c>
       <c r="I24" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J24" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C25" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D25" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E25" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>177</v>
+        <v>147</v>
       </c>
       <c r="G25" t="s">
-        <v>222</v>
+        <v>96</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>241</v>
+        <v>139</v>
       </c>
       <c r="I25" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J25" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C26" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="D26" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E26" t="s">
-        <v>110</v>
-      </c>
-      <c r="F26" t="s">
-        <v>110</v>
+        <v>105</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>148</v>
       </c>
       <c r="G26" t="s">
-        <v>110</v>
-      </c>
-      <c r="H26" t="s">
-        <v>110</v>
+        <v>96</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>139</v>
       </c>
       <c r="I26" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J26" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="27" spans="1:10">
       <c r="A27" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B27" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C27" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="D27" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="E27" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>178</v>
+        <v>149</v>
       </c>
       <c r="G27" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="I27" t="s">
-        <v>255</v>
+        <v>205</v>
       </c>
       <c r="J27" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="28" spans="1:10">
       <c r="A28" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B28" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C28" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D28" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="E28" t="s">
+        <v>107</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G28" t="s">
         <v>126</v>
       </c>
-      <c r="F28" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="G28" t="s">
-        <v>223</v>
-      </c>
       <c r="H28" s="2" t="s">
-        <v>242</v>
+        <v>169</v>
       </c>
       <c r="I28" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J28" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="29" spans="1:10">
       <c r="A29" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B29" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C29" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D29" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E29" t="s">
-        <v>127</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>180</v>
+        <v>93</v>
+      </c>
+      <c r="F29" t="s">
+        <v>93</v>
       </c>
       <c r="G29" t="s">
-        <v>224</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>243</v>
+        <v>93</v>
+      </c>
+      <c r="H29" t="s">
+        <v>93</v>
       </c>
       <c r="I29" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J29" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="30" spans="1:10">
       <c r="A30" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B30" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C30" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D30" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E30" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="F30" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="G30" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="H30" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="I30" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J30" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B31" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C31" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D31" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="E31" t="s">
-        <v>110</v>
-      </c>
-      <c r="F31" t="s">
-        <v>110</v>
+        <v>108</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="G31" t="s">
-        <v>110</v>
-      </c>
-      <c r="H31" t="s">
-        <v>110</v>
+        <v>122</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>165</v>
       </c>
       <c r="I31" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J31" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="32" spans="1:10">
       <c r="A32" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B32" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C32" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D32" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="E32" t="s">
-        <v>110</v>
-      </c>
-      <c r="F32" t="s">
-        <v>110</v>
+        <v>109</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="G32" t="s">
-        <v>110</v>
-      </c>
-      <c r="H32" t="s">
-        <v>110</v>
+        <v>122</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>165</v>
       </c>
       <c r="I32" t="s">
-        <v>255</v>
+        <v>205</v>
       </c>
       <c r="J32" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="33" spans="1:10">
       <c r="A33" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B33" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C33" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D33" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="E33" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>181</v>
+        <v>153</v>
       </c>
       <c r="G33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="I33" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J33" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="34" spans="1:10">
       <c r="A34" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B34" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C34" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D34" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="E34" t="s">
-        <v>129</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>182</v>
+        <v>93</v>
+      </c>
+      <c r="F34" t="s">
+        <v>93</v>
       </c>
       <c r="G34" t="s">
-        <v>118</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>171</v>
+        <v>93</v>
+      </c>
+      <c r="H34" t="s">
+        <v>93</v>
       </c>
       <c r="I34" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J34" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="35" spans="1:10">
       <c r="A35" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B35" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C35" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D35" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="E35" t="s">
+        <v>111</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="G35" t="s">
         <v>130</v>
       </c>
-      <c r="F35" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="G35" t="s">
-        <v>118</v>
-      </c>
       <c r="H35" s="2" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="I35" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J35" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="36" spans="1:10">
       <c r="A36" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B36" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C36" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D36" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E36" t="s">
-        <v>110</v>
-      </c>
-      <c r="F36" t="s">
-        <v>110</v>
+        <v>112</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>155</v>
       </c>
       <c r="G36" t="s">
-        <v>110</v>
-      </c>
-      <c r="H36" t="s">
-        <v>110</v>
+        <v>184</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>198</v>
       </c>
       <c r="I36" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J36" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="37" spans="1:10">
       <c r="A37" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B37" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C37" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="D37" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E37" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>184</v>
+        <v>156</v>
       </c>
       <c r="G37" t="s">
-        <v>156</v>
+        <v>125</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>209</v>
+        <v>168</v>
       </c>
       <c r="I37" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J37" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="38" spans="1:10">
       <c r="A38" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B38" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C38" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="D38" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="E38" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="F38" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="G38" t="s">
         <v>185</v>
       </c>
-      <c r="G38" t="s">
-        <v>225</v>
-      </c>
       <c r="H38" s="2" t="s">
-        <v>244</v>
+        <v>199</v>
       </c>
       <c r="I38" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J38" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B39" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C39" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D39" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E39" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>186</v>
+        <v>158</v>
       </c>
       <c r="G39" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>209</v>
+        <v>167</v>
       </c>
       <c r="I39" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J39" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B40" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C40" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D40" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E40" t="s">
-        <v>110</v>
-      </c>
-      <c r="F40" t="s">
-        <v>110</v>
+        <v>116</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>159</v>
       </c>
       <c r="G40" t="s">
-        <v>110</v>
-      </c>
-      <c r="H40" t="s">
-        <v>110</v>
+        <v>123</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>166</v>
       </c>
       <c r="I40" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J40" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B41" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C41" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D41" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="E41" t="s">
-        <v>134</v>
-      </c>
-      <c r="F41" s="2" t="s">
-        <v>187</v>
+        <v>93</v>
+      </c>
+      <c r="F41" t="s">
+        <v>93</v>
       </c>
       <c r="G41" t="s">
-        <v>152</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>205</v>
+        <v>93</v>
+      </c>
+      <c r="H41" t="s">
+        <v>93</v>
       </c>
       <c r="I41" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J41" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B42" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C42" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="D42" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E42" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="G42" t="s">
-        <v>152</v>
+        <v>127</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>205</v>
+        <v>170</v>
       </c>
       <c r="I42" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J42" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B43" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C43" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="D43" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E43" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>189</v>
+        <v>161</v>
       </c>
       <c r="G43" t="s">
-        <v>137</v>
+        <v>186</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="I43" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J43" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="B44" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C44" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="D44" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="E44" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>190</v>
+        <v>162</v>
       </c>
       <c r="G44" t="s">
-        <v>146</v>
+        <v>187</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="I44" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J44" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B45" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C45" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D45" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E45" t="s">
-        <v>110</v>
-      </c>
-      <c r="F45" t="s">
-        <v>110</v>
+        <v>120</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>163</v>
       </c>
       <c r="G45" t="s">
-        <v>110</v>
-      </c>
-      <c r="H45" t="s">
-        <v>110</v>
+        <v>108</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>151</v>
       </c>
       <c r="I45" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J45" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B46" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C46" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D46" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="E46" t="s">
-        <v>110</v>
-      </c>
-      <c r="F46" t="s">
-        <v>110</v>
+        <v>121</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>164</v>
       </c>
       <c r="G46" t="s">
-        <v>110</v>
-      </c>
-      <c r="H46" t="s">
-        <v>110</v>
+        <v>132</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>175</v>
       </c>
       <c r="I46" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J46" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B47" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C47" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D47" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="E47" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>191</v>
+        <v>165</v>
       </c>
       <c r="G47" t="s">
-        <v>160</v>
+        <v>111</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>213</v>
+        <v>154</v>
       </c>
       <c r="I47" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J47" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B48" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C48" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="D48" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="E48" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>192</v>
+        <v>166</v>
       </c>
       <c r="G48" t="s">
-        <v>138</v>
+        <v>113</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>191</v>
+        <v>156</v>
       </c>
       <c r="I48" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J48" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="49" spans="1:10">
       <c r="A49" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B49" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C49" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D49" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="E49" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>193</v>
+        <v>167</v>
       </c>
       <c r="G49" t="s">
-        <v>226</v>
+        <v>188</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>245</v>
+        <v>202</v>
       </c>
       <c r="I49" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J49" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="50" spans="1:10">
       <c r="A50" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B50" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C50" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D50" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="E50" t="s">
-        <v>110</v>
-      </c>
-      <c r="F50" t="s">
-        <v>110</v>
+        <v>114</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>157</v>
       </c>
       <c r="G50" t="s">
-        <v>110</v>
-      </c>
-      <c r="H50" t="s">
-        <v>110</v>
+        <v>189</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>203</v>
       </c>
       <c r="I50" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J50" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="51" spans="1:10">
       <c r="A51" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B51" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C51" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D51" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="E51" t="s">
-        <v>141</v>
-      </c>
-      <c r="F51" s="2" t="s">
-        <v>194</v>
+        <v>93</v>
+      </c>
+      <c r="F51" t="s">
+        <v>93</v>
       </c>
       <c r="G51" t="s">
-        <v>227</v>
-      </c>
-      <c r="H51" s="2" t="s">
-        <v>246</v>
+        <v>93</v>
+      </c>
+      <c r="H51" t="s">
+        <v>93</v>
       </c>
       <c r="I51" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J51" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B52" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C52" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D52" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="E52" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>195</v>
+        <v>168</v>
       </c>
       <c r="G52" t="s">
-        <v>155</v>
+        <v>110</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>208</v>
+        <v>153</v>
       </c>
       <c r="I52" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J52" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="53" spans="1:10">
       <c r="A53" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B53" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C53" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D53" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="E53" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>196</v>
+        <v>169</v>
       </c>
       <c r="G53" t="s">
-        <v>228</v>
+        <v>121</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>247</v>
+        <v>164</v>
       </c>
       <c r="I53" t="s">
-        <v>255</v>
+        <v>205</v>
       </c>
       <c r="J53" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="54" spans="1:10">
       <c r="A54" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B54" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C54" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="D54" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="E54" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>197</v>
+        <v>170</v>
       </c>
       <c r="G54" t="s">
-        <v>154</v>
+        <v>121</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>207</v>
+        <v>164</v>
       </c>
       <c r="I54" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J54" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="55" spans="1:10">
       <c r="A55" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B55" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C55" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D55" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="E55" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>198</v>
+        <v>171</v>
       </c>
       <c r="G55" t="s">
-        <v>153</v>
+        <v>181</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="I55" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J55" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="56" spans="1:10">
       <c r="A56" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B56" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C56" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="D56" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="E56" t="s">
-        <v>110</v>
-      </c>
-      <c r="F56" t="s">
-        <v>110</v>
+        <v>129</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>172</v>
       </c>
       <c r="G56" t="s">
-        <v>110</v>
-      </c>
-      <c r="H56" t="s">
-        <v>110</v>
+        <v>190</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>204</v>
       </c>
       <c r="I56" t="s">
-        <v>255</v>
+        <v>205</v>
       </c>
       <c r="J56" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="57" spans="1:10">
       <c r="A57" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B57" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="C57" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="D57" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="E57" t="s">
-        <v>110</v>
-      </c>
-      <c r="F57" t="s">
-        <v>110</v>
+        <v>130</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>173</v>
       </c>
       <c r="G57" t="s">
-        <v>110</v>
-      </c>
-      <c r="H57" t="s">
-        <v>110</v>
+        <v>131</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>174</v>
       </c>
       <c r="I57" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J57" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="58" spans="1:10">
       <c r="A58" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B58" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C58" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D58" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="E58" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>199</v>
+        <v>174</v>
       </c>
       <c r="G58" t="s">
-        <v>157</v>
+        <v>128</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>210</v>
+        <v>171</v>
       </c>
       <c r="I58" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J58" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="59" spans="1:10">
       <c r="A59" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B59" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C59" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="D59" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="E59" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>200</v>
+        <v>175</v>
       </c>
       <c r="G59" t="s">
-        <v>229</v>
+        <v>120</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>248</v>
+        <v>163</v>
       </c>
       <c r="I59" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J59" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="60" spans="1:10">
       <c r="A60" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B60" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C60" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D60" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="E60" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>201</v>
+        <v>176</v>
       </c>
       <c r="G60" t="s">
-        <v>230</v>
+        <v>120</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>249</v>
+        <v>163</v>
       </c>
       <c r="I60" t="s">
-        <v>255</v>
+        <v>205</v>
       </c>
       <c r="J60" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
     <row r="61" spans="1:10">
       <c r="A61" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B61" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C61" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D61" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="E61" t="s">
-        <v>149</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>202</v>
+        <v>93</v>
+      </c>
+      <c r="F61" t="s">
+        <v>93</v>
       </c>
       <c r="G61" t="s">
-        <v>231</v>
-      </c>
-      <c r="H61" s="2" t="s">
-        <v>250</v>
+        <v>93</v>
+      </c>
+      <c r="H61" t="s">
+        <v>93</v>
       </c>
       <c r="I61" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="J61" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10">
-      <c r="A62" t="s">
-        <v>28</v>
-      </c>
-      <c r="B62" t="s">
-        <v>51</v>
-      </c>
-      <c r="C62" t="s">
-        <v>72</v>
-      </c>
-      <c r="D62" t="s">
-        <v>99</v>
-      </c>
-      <c r="E62" t="s">
-        <v>150</v>
-      </c>
-      <c r="F62" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="G62" t="s">
-        <v>134</v>
-      </c>
-      <c r="H62" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="I62" t="s">
-        <v>255</v>
-      </c>
-      <c r="J62" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10">
-      <c r="A63" t="s">
-        <v>28</v>
-      </c>
-      <c r="B63" t="s">
-        <v>51</v>
-      </c>
-      <c r="C63" t="s">
-        <v>72</v>
-      </c>
-      <c r="D63" t="s">
-        <v>99</v>
-      </c>
-      <c r="E63" t="s">
-        <v>151</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="G63" t="s">
-        <v>162</v>
-      </c>
-      <c r="H63" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="I63" t="s">
-        <v>255</v>
-      </c>
-      <c r="J63" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10">
-      <c r="A64" t="s">
-        <v>28</v>
-      </c>
-      <c r="B64" t="s">
-        <v>51</v>
-      </c>
-      <c r="C64" t="s">
-        <v>72</v>
-      </c>
-      <c r="D64" t="s">
-        <v>99</v>
-      </c>
-      <c r="E64" t="s">
-        <v>152</v>
-      </c>
-      <c r="F64" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="G64" t="s">
-        <v>138</v>
-      </c>
-      <c r="H64" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="I64" t="s">
-        <v>255</v>
-      </c>
-      <c r="J64" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10">
-      <c r="A65" t="s">
-        <v>29</v>
-      </c>
-      <c r="B65" t="s">
-        <v>52</v>
-      </c>
-      <c r="C65" t="s">
-        <v>72</v>
-      </c>
-      <c r="D65" t="s">
-        <v>99</v>
-      </c>
-      <c r="E65" t="s">
-        <v>153</v>
-      </c>
-      <c r="F65" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="G65" t="s">
-        <v>142</v>
-      </c>
-      <c r="H65" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="I65" t="s">
-        <v>255</v>
-      </c>
-      <c r="J65" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10">
-      <c r="A66" t="s">
-        <v>29</v>
-      </c>
-      <c r="B66" t="s">
-        <v>52</v>
-      </c>
-      <c r="C66" t="s">
-        <v>78</v>
-      </c>
-      <c r="D66" t="s">
-        <v>105</v>
-      </c>
-      <c r="E66" t="s">
-        <v>154</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="G66" t="s">
-        <v>232</v>
-      </c>
-      <c r="H66" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="I66" t="s">
-        <v>255</v>
-      </c>
-      <c r="J66" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10">
-      <c r="A67" t="s">
-        <v>29</v>
-      </c>
-      <c r="B67" t="s">
-        <v>52</v>
-      </c>
-      <c r="C67" t="s">
-        <v>57</v>
-      </c>
-      <c r="D67" t="s">
-        <v>84</v>
-      </c>
-      <c r="E67" t="s">
-        <v>143</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="G67" t="s">
-        <v>233</v>
-      </c>
-      <c r="H67" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="I67" t="s">
-        <v>255</v>
-      </c>
-      <c r="J67" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10">
-      <c r="A68" t="s">
-        <v>30</v>
-      </c>
-      <c r="B68" t="s">
-        <v>53</v>
-      </c>
-      <c r="C68" t="s">
-        <v>72</v>
-      </c>
-      <c r="D68" t="s">
-        <v>99</v>
-      </c>
-      <c r="E68" t="s">
-        <v>155</v>
-      </c>
-      <c r="F68" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="G68" t="s">
-        <v>137</v>
-      </c>
-      <c r="H68" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="I68" t="s">
-        <v>255</v>
-      </c>
-      <c r="J68" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10">
-      <c r="A69" t="s">
-        <v>30</v>
-      </c>
-      <c r="B69" t="s">
-        <v>53</v>
-      </c>
-      <c r="C69" t="s">
-        <v>58</v>
-      </c>
-      <c r="D69" t="s">
-        <v>85</v>
-      </c>
-      <c r="E69" t="s">
-        <v>156</v>
-      </c>
-      <c r="F69" s="2" t="s">
-        <v>209</v>
-      </c>
-      <c r="G69" t="s">
-        <v>151</v>
-      </c>
-      <c r="H69" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="I69" t="s">
-        <v>255</v>
-      </c>
-      <c r="J69" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10">
-      <c r="A70" t="s">
-        <v>30</v>
-      </c>
-      <c r="B70" t="s">
-        <v>53</v>
-      </c>
-      <c r="C70" t="s">
-        <v>72</v>
-      </c>
-      <c r="D70" t="s">
-        <v>99</v>
-      </c>
-      <c r="E70" t="s">
-        <v>157</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="G70" t="s">
-        <v>151</v>
-      </c>
-      <c r="H70" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="I70" t="s">
-        <v>255</v>
-      </c>
-      <c r="J70" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10">
-      <c r="A71" t="s">
-        <v>30</v>
-      </c>
-      <c r="B71" t="s">
-        <v>53</v>
-      </c>
-      <c r="C71" t="s">
-        <v>67</v>
-      </c>
-      <c r="D71" t="s">
-        <v>94</v>
-      </c>
-      <c r="E71" t="s">
-        <v>110</v>
-      </c>
-      <c r="F71" t="s">
-        <v>110</v>
-      </c>
-      <c r="G71" t="s">
-        <v>110</v>
-      </c>
-      <c r="H71" t="s">
-        <v>110</v>
-      </c>
-      <c r="I71" t="s">
-        <v>255</v>
-      </c>
-      <c r="J71" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10">
-      <c r="A72" t="s">
-        <v>31</v>
-      </c>
-      <c r="B72" t="s">
-        <v>54</v>
-      </c>
-      <c r="C72" t="s">
-        <v>79</v>
-      </c>
-      <c r="D72" t="s">
-        <v>106</v>
-      </c>
-      <c r="E72" t="s">
-        <v>158</v>
-      </c>
-      <c r="F72" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="G72" t="s">
-        <v>222</v>
-      </c>
-      <c r="H72" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="I72" t="s">
-        <v>255</v>
-      </c>
-      <c r="J72" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10">
-      <c r="A73" t="s">
-        <v>31</v>
-      </c>
-      <c r="B73" t="s">
-        <v>54</v>
-      </c>
-      <c r="C73" t="s">
-        <v>58</v>
-      </c>
-      <c r="D73" t="s">
-        <v>85</v>
-      </c>
-      <c r="E73" t="s">
-        <v>159</v>
-      </c>
-      <c r="F73" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="G73" t="s">
-        <v>234</v>
-      </c>
-      <c r="H73" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="I73" t="s">
-        <v>255</v>
-      </c>
-      <c r="J73" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10">
-      <c r="A74" t="s">
-        <v>31</v>
-      </c>
-      <c r="B74" t="s">
-        <v>54</v>
-      </c>
-      <c r="C74" t="s">
-        <v>72</v>
-      </c>
-      <c r="D74" t="s">
-        <v>99</v>
-      </c>
-      <c r="E74" t="s">
-        <v>160</v>
-      </c>
-      <c r="F74" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="G74" t="s">
-        <v>161</v>
-      </c>
-      <c r="H74" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="I74" t="s">
-        <v>255</v>
-      </c>
-      <c r="J74" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10">
-      <c r="A75" t="s">
-        <v>31</v>
-      </c>
-      <c r="B75" t="s">
-        <v>54</v>
-      </c>
-      <c r="C75" t="s">
-        <v>80</v>
-      </c>
-      <c r="D75" t="s">
-        <v>107</v>
-      </c>
-      <c r="E75" t="s">
-        <v>161</v>
-      </c>
-      <c r="F75" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="G75" t="s">
-        <v>158</v>
-      </c>
-      <c r="H75" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="I75" t="s">
-        <v>255</v>
-      </c>
-      <c r="J75" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10">
-      <c r="A76" t="s">
-        <v>32</v>
-      </c>
-      <c r="B76" t="s">
-        <v>55</v>
-      </c>
-      <c r="C76" t="s">
-        <v>72</v>
-      </c>
-      <c r="D76" t="s">
-        <v>99</v>
-      </c>
-      <c r="E76" t="s">
-        <v>162</v>
-      </c>
-      <c r="F76" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="G76" t="s">
-        <v>150</v>
-      </c>
-      <c r="H76" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="I76" t="s">
-        <v>255</v>
-      </c>
-      <c r="J76" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10">
-      <c r="A77" t="s">
-        <v>32</v>
-      </c>
-      <c r="B77" t="s">
-        <v>55</v>
-      </c>
-      <c r="C77" t="s">
-        <v>58</v>
-      </c>
-      <c r="D77" t="s">
-        <v>85</v>
-      </c>
-      <c r="E77" t="s">
-        <v>163</v>
-      </c>
-      <c r="F77" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="G77" t="s">
-        <v>150</v>
-      </c>
-      <c r="H77" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="I77" t="s">
-        <v>255</v>
-      </c>
-      <c r="J77" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10">
-      <c r="A78" t="s">
-        <v>32</v>
-      </c>
-      <c r="B78" t="s">
-        <v>55</v>
-      </c>
-      <c r="C78" t="s">
-        <v>81</v>
-      </c>
-      <c r="D78" t="s">
-        <v>108</v>
-      </c>
-      <c r="E78" t="s">
-        <v>148</v>
-      </c>
-      <c r="F78" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="G78" t="s">
-        <v>235</v>
-      </c>
-      <c r="H78" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="I78" t="s">
-        <v>255</v>
-      </c>
-      <c r="J78" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10">
-      <c r="A79" t="s">
-        <v>32</v>
-      </c>
-      <c r="B79" t="s">
-        <v>55</v>
-      </c>
-      <c r="C79" t="s">
-        <v>82</v>
-      </c>
-      <c r="D79" t="s">
-        <v>109</v>
-      </c>
-      <c r="E79" t="s">
-        <v>110</v>
-      </c>
-      <c r="F79" t="s">
-        <v>110</v>
-      </c>
-      <c r="G79" t="s">
-        <v>110</v>
-      </c>
-      <c r="H79" t="s">
-        <v>110</v>
-      </c>
-      <c r="I79" t="s">
-        <v>255</v>
-      </c>
-      <c r="J79" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F4" r:id="rId1"/>
-    <hyperlink ref="H4" r:id="rId2"/>
-    <hyperlink ref="F5" r:id="rId3"/>
-    <hyperlink ref="H5" r:id="rId4"/>
-    <hyperlink ref="F6" r:id="rId5"/>
-    <hyperlink ref="H6" r:id="rId6"/>
-    <hyperlink ref="F7" r:id="rId7"/>
-    <hyperlink ref="H7" r:id="rId8"/>
-    <hyperlink ref="F8" r:id="rId9"/>
-    <hyperlink ref="H8" r:id="rId10"/>
-    <hyperlink ref="F12" r:id="rId11"/>
-    <hyperlink ref="H12" r:id="rId12"/>
-    <hyperlink ref="F13" r:id="rId13"/>
-    <hyperlink ref="H13" r:id="rId14"/>
-    <hyperlink ref="F14" r:id="rId15"/>
-    <hyperlink ref="H14" r:id="rId16"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="H2" r:id="rId2"/>
+    <hyperlink ref="F3" r:id="rId3"/>
+    <hyperlink ref="H3" r:id="rId4"/>
+    <hyperlink ref="F4" r:id="rId5"/>
+    <hyperlink ref="H4" r:id="rId6"/>
+    <hyperlink ref="F6" r:id="rId7"/>
+    <hyperlink ref="H6" r:id="rId8"/>
+    <hyperlink ref="F9" r:id="rId9"/>
+    <hyperlink ref="H9" r:id="rId10"/>
+    <hyperlink ref="F10" r:id="rId11"/>
+    <hyperlink ref="H10" r:id="rId12"/>
+    <hyperlink ref="F12" r:id="rId13"/>
+    <hyperlink ref="H12" r:id="rId14"/>
+    <hyperlink ref="F13" r:id="rId15"/>
+    <hyperlink ref="H13" r:id="rId16"/>
     <hyperlink ref="F15" r:id="rId17"/>
     <hyperlink ref="H15" r:id="rId18"/>
     <hyperlink ref="F17" r:id="rId19"/>
@@ -3714,92 +2991,70 @@
     <hyperlink ref="H20" r:id="rId24"/>
     <hyperlink ref="F21" r:id="rId25"/>
     <hyperlink ref="H21" r:id="rId26"/>
-    <hyperlink ref="F24" r:id="rId27"/>
-    <hyperlink ref="H24" r:id="rId28"/>
+    <hyperlink ref="F22" r:id="rId27"/>
+    <hyperlink ref="H22" r:id="rId28"/>
     <hyperlink ref="F25" r:id="rId29"/>
     <hyperlink ref="H25" r:id="rId30"/>
-    <hyperlink ref="F27" r:id="rId31"/>
-    <hyperlink ref="H27" r:id="rId32"/>
-    <hyperlink ref="F28" r:id="rId33"/>
-    <hyperlink ref="H28" r:id="rId34"/>
-    <hyperlink ref="F29" r:id="rId35"/>
-    <hyperlink ref="H29" r:id="rId36"/>
-    <hyperlink ref="F33" r:id="rId37"/>
-    <hyperlink ref="H33" r:id="rId38"/>
-    <hyperlink ref="F34" r:id="rId39"/>
-    <hyperlink ref="H34" r:id="rId40"/>
-    <hyperlink ref="F35" r:id="rId41"/>
-    <hyperlink ref="H35" r:id="rId42"/>
-    <hyperlink ref="F37" r:id="rId43"/>
-    <hyperlink ref="H37" r:id="rId44"/>
-    <hyperlink ref="F38" r:id="rId45"/>
-    <hyperlink ref="H38" r:id="rId46"/>
-    <hyperlink ref="F39" r:id="rId47"/>
-    <hyperlink ref="H39" r:id="rId48"/>
-    <hyperlink ref="F41" r:id="rId49"/>
-    <hyperlink ref="H41" r:id="rId50"/>
-    <hyperlink ref="F42" r:id="rId51"/>
-    <hyperlink ref="H42" r:id="rId52"/>
-    <hyperlink ref="F43" r:id="rId53"/>
-    <hyperlink ref="H43" r:id="rId54"/>
-    <hyperlink ref="F44" r:id="rId55"/>
-    <hyperlink ref="H44" r:id="rId56"/>
-    <hyperlink ref="F47" r:id="rId57"/>
-    <hyperlink ref="H47" r:id="rId58"/>
-    <hyperlink ref="F48" r:id="rId59"/>
-    <hyperlink ref="H48" r:id="rId60"/>
-    <hyperlink ref="F49" r:id="rId61"/>
-    <hyperlink ref="H49" r:id="rId62"/>
-    <hyperlink ref="F51" r:id="rId63"/>
-    <hyperlink ref="H51" r:id="rId64"/>
-    <hyperlink ref="F52" r:id="rId65"/>
-    <hyperlink ref="H52" r:id="rId66"/>
-    <hyperlink ref="F53" r:id="rId67"/>
-    <hyperlink ref="H53" r:id="rId68"/>
-    <hyperlink ref="F54" r:id="rId69"/>
-    <hyperlink ref="H54" r:id="rId70"/>
-    <hyperlink ref="F55" r:id="rId71"/>
-    <hyperlink ref="H55" r:id="rId72"/>
-    <hyperlink ref="F58" r:id="rId73"/>
-    <hyperlink ref="H58" r:id="rId74"/>
-    <hyperlink ref="F59" r:id="rId75"/>
-    <hyperlink ref="H59" r:id="rId76"/>
-    <hyperlink ref="F60" r:id="rId77"/>
-    <hyperlink ref="H60" r:id="rId78"/>
-    <hyperlink ref="F61" r:id="rId79"/>
-    <hyperlink ref="H61" r:id="rId80"/>
-    <hyperlink ref="F62" r:id="rId81"/>
-    <hyperlink ref="H62" r:id="rId82"/>
-    <hyperlink ref="F63" r:id="rId83"/>
-    <hyperlink ref="H63" r:id="rId84"/>
-    <hyperlink ref="F64" r:id="rId85"/>
-    <hyperlink ref="H64" r:id="rId86"/>
-    <hyperlink ref="F65" r:id="rId87"/>
-    <hyperlink ref="H65" r:id="rId88"/>
-    <hyperlink ref="F66" r:id="rId89"/>
-    <hyperlink ref="H66" r:id="rId90"/>
-    <hyperlink ref="F67" r:id="rId91"/>
-    <hyperlink ref="H67" r:id="rId92"/>
-    <hyperlink ref="F68" r:id="rId93"/>
-    <hyperlink ref="H68" r:id="rId94"/>
-    <hyperlink ref="F69" r:id="rId95"/>
-    <hyperlink ref="H69" r:id="rId96"/>
-    <hyperlink ref="F70" r:id="rId97"/>
-    <hyperlink ref="H70" r:id="rId98"/>
-    <hyperlink ref="F72" r:id="rId99"/>
-    <hyperlink ref="H72" r:id="rId100"/>
-    <hyperlink ref="F73" r:id="rId101"/>
-    <hyperlink ref="H73" r:id="rId102"/>
-    <hyperlink ref="F74" r:id="rId103"/>
-    <hyperlink ref="H74" r:id="rId104"/>
-    <hyperlink ref="F75" r:id="rId105"/>
-    <hyperlink ref="H75" r:id="rId106"/>
-    <hyperlink ref="F76" r:id="rId107"/>
-    <hyperlink ref="H76" r:id="rId108"/>
-    <hyperlink ref="F77" r:id="rId109"/>
-    <hyperlink ref="H77" r:id="rId110"/>
-    <hyperlink ref="F78" r:id="rId111"/>
-    <hyperlink ref="H78" r:id="rId112"/>
+    <hyperlink ref="F26" r:id="rId31"/>
+    <hyperlink ref="H26" r:id="rId32"/>
+    <hyperlink ref="F27" r:id="rId33"/>
+    <hyperlink ref="H27" r:id="rId34"/>
+    <hyperlink ref="F28" r:id="rId35"/>
+    <hyperlink ref="H28" r:id="rId36"/>
+    <hyperlink ref="F31" r:id="rId37"/>
+    <hyperlink ref="H31" r:id="rId38"/>
+    <hyperlink ref="F32" r:id="rId39"/>
+    <hyperlink ref="H32" r:id="rId40"/>
+    <hyperlink ref="F33" r:id="rId41"/>
+    <hyperlink ref="H33" r:id="rId42"/>
+    <hyperlink ref="F35" r:id="rId43"/>
+    <hyperlink ref="H35" r:id="rId44"/>
+    <hyperlink ref="F36" r:id="rId45"/>
+    <hyperlink ref="H36" r:id="rId46"/>
+    <hyperlink ref="F37" r:id="rId47"/>
+    <hyperlink ref="H37" r:id="rId48"/>
+    <hyperlink ref="F38" r:id="rId49"/>
+    <hyperlink ref="H38" r:id="rId50"/>
+    <hyperlink ref="F39" r:id="rId51"/>
+    <hyperlink ref="H39" r:id="rId52"/>
+    <hyperlink ref="F40" r:id="rId53"/>
+    <hyperlink ref="H40" r:id="rId54"/>
+    <hyperlink ref="F42" r:id="rId55"/>
+    <hyperlink ref="H42" r:id="rId56"/>
+    <hyperlink ref="F43" r:id="rId57"/>
+    <hyperlink ref="H43" r:id="rId58"/>
+    <hyperlink ref="F44" r:id="rId59"/>
+    <hyperlink ref="H44" r:id="rId60"/>
+    <hyperlink ref="F45" r:id="rId61"/>
+    <hyperlink ref="H45" r:id="rId62"/>
+    <hyperlink ref="F46" r:id="rId63"/>
+    <hyperlink ref="H46" r:id="rId64"/>
+    <hyperlink ref="F47" r:id="rId65"/>
+    <hyperlink ref="H47" r:id="rId66"/>
+    <hyperlink ref="F48" r:id="rId67"/>
+    <hyperlink ref="H48" r:id="rId68"/>
+    <hyperlink ref="F49" r:id="rId69"/>
+    <hyperlink ref="H49" r:id="rId70"/>
+    <hyperlink ref="F50" r:id="rId71"/>
+    <hyperlink ref="H50" r:id="rId72"/>
+    <hyperlink ref="F52" r:id="rId73"/>
+    <hyperlink ref="H52" r:id="rId74"/>
+    <hyperlink ref="F53" r:id="rId75"/>
+    <hyperlink ref="H53" r:id="rId76"/>
+    <hyperlink ref="F54" r:id="rId77"/>
+    <hyperlink ref="H54" r:id="rId78"/>
+    <hyperlink ref="F55" r:id="rId79"/>
+    <hyperlink ref="H55" r:id="rId80"/>
+    <hyperlink ref="F56" r:id="rId81"/>
+    <hyperlink ref="H56" r:id="rId82"/>
+    <hyperlink ref="F57" r:id="rId83"/>
+    <hyperlink ref="H57" r:id="rId84"/>
+    <hyperlink ref="F58" r:id="rId85"/>
+    <hyperlink ref="H58" r:id="rId86"/>
+    <hyperlink ref="F59" r:id="rId87"/>
+    <hyperlink ref="H59" r:id="rId88"/>
+    <hyperlink ref="F60" r:id="rId89"/>
+    <hyperlink ref="H60" r:id="rId90"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>